<commit_message>
Add new combinations - TMY2020 and TMYA01.
</commit_message>
<xml_diff>
--- a/Combinations.xlsx
+++ b/Combinations.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayala\Documents\GitHub\Studies\Approaches2BifacialPerformanceMonitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C50D301-7E89-45F1-8900-C609351BF706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3791C5-5F2E-486D-97AA-AC01D6699560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A009557A-D0E6-45B8-942A-C4AB4B72D0E6}"/>
+    <workbookView xWindow="-28920" yWindow="-6360" windowWidth="29040" windowHeight="15840" xr2:uid="{A009557A-D0E6-45B8-942A-C4AB4B72D0E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="184">
   <si>
     <t>Input Variables</t>
   </si>
@@ -574,6 +573,21 @@
   </si>
   <si>
     <t>TrackerAngle</t>
+  </si>
+  <si>
+    <t>TMY2020</t>
+  </si>
+  <si>
+    <t>NSRDB</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>TMY + Albedo (method1)</t>
+  </si>
+  <si>
+    <t>TMYA01</t>
   </si>
 </sst>
 </file>
@@ -895,6 +909,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -918,24 +950,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1256,34 +1270,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F903F77-CC72-401E-A0BD-CC4B63665887}">
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="40.85546875" customWidth="1"/>
-    <col min="9" max="10" width="51.42578125" customWidth="1"/>
-    <col min="11" max="11" width="34.140625" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" customWidth="1"/>
-    <col min="13" max="13" width="44.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="46.5703125" customWidth="1"/>
-    <col min="16" max="16" width="26.85546875" customWidth="1"/>
-    <col min="17" max="18" width="21.85546875" customWidth="1"/>
-    <col min="19" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="18.85546875" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="40.88671875" customWidth="1"/>
+    <col min="9" max="10" width="51.44140625" customWidth="1"/>
+    <col min="11" max="11" width="42.88671875" customWidth="1"/>
+    <col min="12" max="12" width="24.6640625" customWidth="1"/>
+    <col min="13" max="13" width="44.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="46.5546875" customWidth="1"/>
+    <col min="16" max="16" width="26.88671875" customWidth="1"/>
+    <col min="17" max="18" width="21.88671875" customWidth="1"/>
+    <col min="19" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="18.88671875" customWidth="1"/>
+    <col min="22" max="22" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>84</v>
       </c>
@@ -1326,14 +1340,14 @@
       <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-    </row>
-    <row r="2" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+    </row>
+    <row r="2" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>85</v>
       </c>
@@ -1380,7 +1394,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H3" s="3" t="s">
         <v>92</v>
       </c>
@@ -1424,7 +1438,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H4" s="3" t="s">
         <v>51</v>
       </c>
@@ -1460,7 +1474,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H5" s="3" t="s">
         <v>52</v>
       </c>
@@ -1490,7 +1504,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H6" s="5" t="s">
         <v>53</v>
       </c>
@@ -1508,7 +1522,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H7" s="3" t="s">
         <v>54</v>
       </c>
@@ -1523,7 +1537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H8" s="5" t="s">
         <v>55</v>
       </c>
@@ -1539,7 +1553,7 @@
       </c>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H9" s="3" t="s">
         <v>56</v>
       </c>
@@ -1554,7 +1568,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H10" s="5" t="s">
         <v>93</v>
       </c>
@@ -1573,7 +1587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:22" x14ac:dyDescent="0.3">
       <c r="H11" s="3" t="s">
         <v>150</v>
       </c>
@@ -1592,7 +1606,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:22" x14ac:dyDescent="0.3">
       <c r="I12" s="5" t="s">
         <v>69</v>
       </c>
@@ -1606,7 +1620,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:22" x14ac:dyDescent="0.3">
       <c r="G13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1620,7 +1634,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:22" x14ac:dyDescent="0.3">
       <c r="G14" s="5" t="s">
         <v>30</v>
       </c>
@@ -1636,7 +1650,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:22" x14ac:dyDescent="0.3">
       <c r="G15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1652,7 +1666,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:22" x14ac:dyDescent="0.3">
       <c r="I16" s="3" t="s">
         <v>73</v>
       </c>
@@ -1664,7 +1678,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="H17" s="8"/>
       <c r="I17" s="3" t="s">
         <v>151</v>
@@ -1674,51 +1688,51 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="26"/>
       <c r="N20" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="O20" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
       <c r="R20" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="S20" s="13" t="s">
+      <c r="S20" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="15"/>
-    </row>
-    <row r="21" spans="1:22" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="21"/>
+    </row>
+    <row r="21" spans="1:22" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>101</v>
       </c>
@@ -1758,7 +1772,7 @@
       <c r="M21" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="N21" s="26" t="s">
+      <c r="N21" s="7" t="s">
         <v>178</v>
       </c>
       <c r="O21" s="7" t="s">
@@ -1786,48 +1800,48 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="25" t="s">
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6">
-        <v>0</v>
-      </c>
-      <c r="J22" s="6">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="G22" t="s">
+        <v>180</v>
+      </c>
+      <c r="H22" t="s">
+        <v>180</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>180</v>
+      </c>
+      <c r="L22" t="s">
+        <v>180</v>
+      </c>
+      <c r="M22" t="s">
+        <v>180</v>
+      </c>
+      <c r="N22" t="s">
+        <v>181</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1839,60 +1853,60 @@
         <v>17</v>
       </c>
       <c r="S22" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="T22" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="U22" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="V22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>100</v>
+        <v>183</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="6">
-        <v>0</v>
-      </c>
-      <c r="I23" s="6">
-        <v>0</v>
-      </c>
-      <c r="J23" s="6">
+        <v>180</v>
+      </c>
+      <c r="G23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H23" t="s">
+        <v>180</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+      <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
+      <c r="L23" t="s">
+        <v>180</v>
+      </c>
+      <c r="M23" t="s">
+        <v>180</v>
+      </c>
+      <c r="N23" t="s">
+        <v>181</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1904,29 +1918,31 @@
         <v>17</v>
       </c>
       <c r="S23" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="T23" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="U23" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="V23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="B24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="23"/>
+      <c r="B24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="E24" t="s">
         <v>27</v>
       </c>
@@ -1946,7 +1962,7 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -1979,17 +1995,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="23"/>
+        <v>86</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="E25" t="s">
         <v>27</v>
       </c>
@@ -2009,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2042,17 +2060,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="23"/>
+        <v>87</v>
+      </c>
+      <c r="D26" s="15"/>
       <c r="E26" t="s">
         <v>27</v>
       </c>
@@ -2072,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -2105,19 +2123,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>110</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D27" s="15"/>
       <c r="E27" t="s">
         <v>27</v>
       </c>
@@ -2137,10 +2153,10 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -2158,10 +2174,10 @@
         <v>17</v>
       </c>
       <c r="S27" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="T27" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="U27" t="s">
         <v>24</v>
@@ -2170,17 +2186,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="23"/>
+        <v>89</v>
+      </c>
+      <c r="D28" s="15"/>
       <c r="E28" t="s">
         <v>27</v>
       </c>
@@ -2200,10 +2216,10 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -2221,10 +2237,10 @@
         <v>17</v>
       </c>
       <c r="S28" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="T28" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="U28" t="s">
         <v>24</v>
@@ -2233,17 +2249,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="23"/>
+        <v>102</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="E29" t="s">
         <v>27</v>
       </c>
@@ -2266,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -2296,19 +2314,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>111</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="D30" s="15"/>
       <c r="E30" t="s">
         <v>27</v>
       </c>
@@ -2331,10 +2347,10 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -2361,17 +2377,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="23"/>
+        <v>104</v>
+      </c>
+      <c r="D31" s="15"/>
       <c r="E31" t="s">
         <v>27</v>
       </c>
@@ -2394,10 +2410,10 @@
         <v>0</v>
       </c>
       <c r="L31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N31">
         <v>0</v>
@@ -2424,17 +2440,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="23"/>
+        <v>106</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>111</v>
+      </c>
       <c r="E32" t="s">
         <v>27</v>
       </c>
@@ -2460,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N32">
         <v>0</v>
@@ -2487,17 +2505,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" s="23"/>
+        <v>107</v>
+      </c>
+      <c r="D33" s="15"/>
       <c r="E33" t="s">
         <v>27</v>
       </c>
@@ -2523,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -2550,19 +2568,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="15"/>
       <c r="E34" t="s">
         <v>27</v>
       </c>
@@ -2588,13 +2604,13 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N34">
         <v>0</v>
       </c>
       <c r="O34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34">
         <v>2</v>
@@ -2603,10 +2619,10 @@
         <v>17</v>
       </c>
       <c r="S34" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="T34" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="U34" t="s">
         <v>24</v>
@@ -2615,17 +2631,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="24"/>
+        <v>109</v>
+      </c>
+      <c r="C35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="15"/>
       <c r="E35" t="s">
         <v>27</v>
       </c>
@@ -2651,13 +2667,13 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N35">
         <v>0</v>
       </c>
       <c r="O35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P35">
         <v>2</v>
@@ -2666,10 +2682,10 @@
         <v>17</v>
       </c>
       <c r="S35" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="T35" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="U35" t="s">
         <v>24</v>
@@ -2678,17 +2694,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="24"/>
+      <c r="D36" s="16" t="s">
+        <v>118</v>
+      </c>
       <c r="E36" t="s">
         <v>27</v>
       </c>
@@ -2720,10 +2738,10 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q36" t="s">
         <v>17</v>
@@ -2741,17 +2759,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="24"/>
+      <c r="D37" s="16"/>
       <c r="E37" t="s">
         <v>27</v>
       </c>
@@ -2783,10 +2801,10 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q37" t="s">
         <v>17</v>
@@ -2804,17 +2822,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="24"/>
+      <c r="D38" s="16"/>
       <c r="E38" t="s">
         <v>27</v>
       </c>
@@ -2846,10 +2864,10 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="s">
         <v>17</v>
@@ -2867,17 +2885,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="24"/>
+      <c r="D39" s="16"/>
       <c r="E39" t="s">
         <v>27</v>
       </c>
@@ -2909,7 +2927,7 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P39">
         <v>1</v>
@@ -2930,19 +2948,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>124</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D40" s="16"/>
       <c r="E40" t="s">
         <v>27</v>
       </c>
@@ -2959,25 +2975,25 @@
         <v>0</v>
       </c>
       <c r="J40" s="6">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
         <v>1</v>
       </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>3</v>
-      </c>
       <c r="P40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q40" t="s">
         <v>17</v>
@@ -2995,17 +3011,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="D41" s="16"/>
       <c r="E41" t="s">
         <v>27</v>
       </c>
@@ -3016,31 +3032,31 @@
         <v>29</v>
       </c>
       <c r="H41" s="6">
+        <v>0</v>
+      </c>
+      <c r="I41" s="6">
+        <v>0</v>
+      </c>
+      <c r="J41" s="6">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>2</v>
+      </c>
+      <c r="P41">
         <v>1</v>
-      </c>
-      <c r="I41" s="6">
-        <v>0</v>
-      </c>
-      <c r="J41" s="6">
-        <v>1</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>3</v>
-      </c>
-      <c r="P41">
-        <v>2</v>
       </c>
       <c r="Q41" t="s">
         <v>17</v>
@@ -3058,17 +3074,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" s="23"/>
+        <v>119</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="E42" t="s">
         <v>27</v>
       </c>
@@ -3079,7 +3097,7 @@
         <v>29</v>
       </c>
       <c r="H42" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I42" s="6">
         <v>0</v>
@@ -3121,17 +3139,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
-      </c>
-      <c r="C43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" s="23"/>
+        <v>120</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="15"/>
       <c r="E43" t="s">
         <v>27</v>
       </c>
@@ -3142,7 +3160,7 @@
         <v>29</v>
       </c>
       <c r="H43" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I43" s="6">
         <v>0</v>
@@ -3184,17 +3202,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="23"/>
+        <v>122</v>
+      </c>
+      <c r="D44" s="15"/>
       <c r="E44" t="s">
         <v>27</v>
       </c>
@@ -3205,7 +3223,7 @@
         <v>29</v>
       </c>
       <c r="H44" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I44" s="6">
         <v>0</v>
@@ -3247,17 +3265,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
-      </c>
-      <c r="D45" s="23"/>
+        <v>125</v>
+      </c>
+      <c r="D45" s="15"/>
       <c r="E45" t="s">
         <v>27</v>
       </c>
@@ -3268,7 +3286,7 @@
         <v>29</v>
       </c>
       <c r="H45" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I45" s="6">
         <v>0</v>
@@ -3310,17 +3328,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
-      </c>
-      <c r="D46" s="23"/>
+        <v>126</v>
+      </c>
+      <c r="D46" s="15"/>
       <c r="E46" t="s">
         <v>27</v>
       </c>
@@ -3331,7 +3349,7 @@
         <v>29</v>
       </c>
       <c r="H46" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I46" s="6">
         <v>0</v>
@@ -3373,19 +3391,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>123</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D47" s="15"/>
       <c r="E47" t="s">
         <v>27</v>
       </c>
@@ -3396,7 +3412,7 @@
         <v>29</v>
       </c>
       <c r="H47" s="6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I47" s="6">
         <v>0</v>
@@ -3417,7 +3433,7 @@
         <v>0</v>
       </c>
       <c r="O47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P47">
         <v>2</v>
@@ -3438,17 +3454,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
-      </c>
-      <c r="D48" s="23"/>
+        <v>128</v>
+      </c>
+      <c r="D48" s="15"/>
       <c r="E48" t="s">
         <v>27</v>
       </c>
@@ -3459,7 +3475,7 @@
         <v>29</v>
       </c>
       <c r="H48" s="6">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I48" s="6">
         <v>0</v>
@@ -3480,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="O48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P48">
         <v>2</v>
@@ -3501,17 +3517,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
-      </c>
-      <c r="D49" s="23"/>
+        <v>129</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>123</v>
+      </c>
       <c r="E49" t="s">
         <v>27</v>
       </c>
@@ -3522,7 +3540,7 @@
         <v>29</v>
       </c>
       <c r="H49" s="6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I49" s="6">
         <v>0</v>
@@ -3564,17 +3582,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
-      </c>
-      <c r="D50" s="23"/>
+        <v>130</v>
+      </c>
+      <c r="D50" s="15"/>
       <c r="E50" t="s">
         <v>27</v>
       </c>
@@ -3585,7 +3603,7 @@
         <v>29</v>
       </c>
       <c r="H50" s="6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I50" s="6">
         <v>0</v>
@@ -3627,19 +3645,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>133</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D51" s="15"/>
       <c r="E51" t="s">
         <v>27</v>
       </c>
@@ -3650,7 +3666,7 @@
         <v>29</v>
       </c>
       <c r="H51" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I51" s="6">
         <v>0</v>
@@ -3692,19 +3708,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>134</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" s="15"/>
       <c r="E52" t="s">
         <v>27</v>
       </c>
@@ -3715,13 +3729,13 @@
         <v>29</v>
       </c>
       <c r="H52" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I52" s="6">
         <v>0</v>
       </c>
       <c r="J52" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -3736,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="O52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P52">
         <v>2</v>
@@ -3757,17 +3771,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
-        <v>136</v>
-      </c>
-      <c r="D53" s="23"/>
+        <v>132</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>133</v>
+      </c>
       <c r="E53" t="s">
         <v>27</v>
       </c>
@@ -3778,14 +3794,14 @@
         <v>29</v>
       </c>
       <c r="H53" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I53" s="6">
+        <v>0</v>
+      </c>
+      <c r="J53" s="6">
         <v>1</v>
       </c>
-      <c r="J53" s="6">
-        <v>2</v>
-      </c>
       <c r="K53">
         <v>0</v>
       </c>
@@ -3799,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="O53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P53">
         <v>2</v>
@@ -3820,17 +3836,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
-      </c>
-      <c r="C54" t="s">
-        <v>137</v>
-      </c>
-      <c r="D54" s="23"/>
+        <v>135</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>134</v>
+      </c>
       <c r="E54" t="s">
         <v>27</v>
       </c>
@@ -3844,7 +3862,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J54" s="6">
         <v>2</v>
@@ -3883,17 +3901,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
-      </c>
-      <c r="D55" s="23"/>
+        <v>136</v>
+      </c>
+      <c r="D55" s="15"/>
       <c r="E55" t="s">
         <v>27</v>
       </c>
@@ -3907,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="I55" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J55" s="6">
         <v>2</v>
@@ -3946,17 +3964,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C56" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" s="23"/>
+        <v>137</v>
+      </c>
+      <c r="D56" s="15"/>
       <c r="E56" t="s">
         <v>27</v>
       </c>
@@ -3970,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J56" s="6">
         <v>2</v>
@@ -4009,17 +4027,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
-      </c>
-      <c r="D57" s="23"/>
+        <v>138</v>
+      </c>
+      <c r="D57" s="15"/>
       <c r="E57" t="s">
         <v>27</v>
       </c>
@@ -4033,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J57" s="6">
         <v>2</v>
@@ -4072,17 +4090,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C58" t="s">
-        <v>144</v>
-      </c>
-      <c r="D58" s="23"/>
+        <v>139</v>
+      </c>
+      <c r="D58" s="15"/>
       <c r="E58" t="s">
         <v>27</v>
       </c>
@@ -4096,7 +4114,7 @@
         <v>0</v>
       </c>
       <c r="I58" s="6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J58" s="6">
         <v>2</v>
@@ -4135,17 +4153,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
-      </c>
-      <c r="D59" s="23"/>
+        <v>143</v>
+      </c>
+      <c r="D59" s="15"/>
       <c r="E59" t="s">
         <v>27</v>
       </c>
@@ -4159,7 +4177,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J59" s="6">
         <v>2</v>
@@ -4198,17 +4216,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" s="23"/>
+        <v>144</v>
+      </c>
+      <c r="D60" s="15"/>
       <c r="E60" t="s">
         <v>27</v>
       </c>
@@ -4222,7 +4240,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J60" s="6">
         <v>2</v>
@@ -4261,17 +4279,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
-      </c>
-      <c r="D61" s="23"/>
+        <v>140</v>
+      </c>
+      <c r="D61" s="15"/>
       <c r="E61" t="s">
         <v>27</v>
       </c>
@@ -4285,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="6">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J61" s="6">
         <v>2</v>
@@ -4324,17 +4342,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>145</v>
-      </c>
-      <c r="D62" s="23"/>
+        <v>141</v>
+      </c>
+      <c r="D62" s="15"/>
       <c r="E62" t="s">
         <v>27</v>
       </c>
@@ -4348,7 +4366,7 @@
         <v>0</v>
       </c>
       <c r="I62" s="6">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J62" s="6">
         <v>2</v>
@@ -4387,17 +4405,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63" s="23"/>
+        <v>142</v>
+      </c>
+      <c r="D63" s="15"/>
       <c r="E63" t="s">
         <v>27</v>
       </c>
@@ -4411,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="6">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J63" s="6">
         <v>2</v>
@@ -4450,17 +4468,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C64" t="s">
-        <v>147</v>
-      </c>
-      <c r="D64" s="23"/>
+        <v>145</v>
+      </c>
+      <c r="D64" s="15"/>
       <c r="E64" t="s">
         <v>27</v>
       </c>
@@ -4471,10 +4489,10 @@
         <v>29</v>
       </c>
       <c r="H64" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I64" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J64" s="6">
         <v>2</v>
@@ -4513,19 +4531,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
-      </c>
-      <c r="D65" s="23" t="s">
-        <v>157</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D65" s="15"/>
       <c r="E65" t="s">
         <v>27</v>
       </c>
@@ -4536,10 +4552,10 @@
         <v>29</v>
       </c>
       <c r="H65" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I65" s="6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J65" s="6">
         <v>2</v>
@@ -4557,7 +4573,7 @@
         <v>0</v>
       </c>
       <c r="O65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P65">
         <v>2</v>
@@ -4578,17 +4594,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
-      </c>
-      <c r="D66" s="23"/>
+        <v>147</v>
+      </c>
+      <c r="D66" s="15"/>
       <c r="E66" t="s">
         <v>27</v>
       </c>
@@ -4599,10 +4615,10 @@
         <v>29</v>
       </c>
       <c r="H66" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I66" s="6">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J66" s="6">
         <v>2</v>
@@ -4620,7 +4636,7 @@
         <v>0</v>
       </c>
       <c r="O66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P66">
         <v>2</v>
@@ -4641,17 +4657,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C67" t="s">
-        <v>153</v>
-      </c>
-      <c r="D67" s="23"/>
+        <v>148</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>157</v>
+      </c>
       <c r="E67" t="s">
         <v>27</v>
       </c>
@@ -4665,7 +4683,7 @@
         <v>10</v>
       </c>
       <c r="I67" s="6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J67" s="6">
         <v>2</v>
@@ -4704,17 +4722,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
-      </c>
-      <c r="D68" s="23"/>
+        <v>149</v>
+      </c>
+      <c r="D68" s="15"/>
       <c r="E68" t="s">
         <v>27</v>
       </c>
@@ -4728,7 +4746,7 @@
         <v>10</v>
       </c>
       <c r="I68" s="6">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="J68" s="6">
         <v>2</v>
@@ -4767,19 +4785,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C69" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>158</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="D69" s="15"/>
       <c r="E69" t="s">
         <v>27</v>
       </c>
@@ -4793,7 +4809,7 @@
         <v>10</v>
       </c>
       <c r="I69" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J69" s="6">
         <v>2</v>
@@ -4832,17 +4848,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
-      </c>
-      <c r="D70" s="23"/>
+        <v>154</v>
+      </c>
+      <c r="D70" s="15"/>
       <c r="E70" t="s">
         <v>27</v>
       </c>
@@ -4853,10 +4869,10 @@
         <v>29</v>
       </c>
       <c r="H70" s="6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I70" s="6">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J70" s="6">
         <v>2</v>
@@ -4895,22 +4911,150 @@
         <v>24</v>
       </c>
     </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" t="s">
+        <v>155</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E71" t="s">
+        <v>27</v>
+      </c>
+      <c r="F71" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H71" s="6">
+        <v>10</v>
+      </c>
+      <c r="I71" s="6">
+        <v>12</v>
+      </c>
+      <c r="J71" s="6">
+        <v>2</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>4</v>
+      </c>
+      <c r="P71">
+        <v>2</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>17</v>
+      </c>
+      <c r="S71" t="s">
+        <v>24</v>
+      </c>
+      <c r="T71" t="s">
+        <v>24</v>
+      </c>
+      <c r="U71" t="s">
+        <v>24</v>
+      </c>
+      <c r="V71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" t="s">
+        <v>156</v>
+      </c>
+      <c r="D72" s="15"/>
+      <c r="E72" t="s">
+        <v>27</v>
+      </c>
+      <c r="F72" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H72" s="6">
+        <v>7</v>
+      </c>
+      <c r="I72" s="6">
+        <v>12</v>
+      </c>
+      <c r="J72" s="6">
+        <v>2</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>4</v>
+      </c>
+      <c r="P72">
+        <v>2</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>17</v>
+      </c>
+      <c r="S72" t="s">
+        <v>24</v>
+      </c>
+      <c r="T72" t="s">
+        <v>24</v>
+      </c>
+      <c r="U72" t="s">
+        <v>24</v>
+      </c>
+      <c r="V72" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D40:D46"/>
-    <mergeCell ref="D52:D64"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="S20:V20"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="O20:Q20"/>
     <mergeCell ref="E20:M20"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="D42:D48"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="D54:D66"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D36:D41"/>
+    <mergeCell ref="D32:D35"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add IEC 5 minute weatherfiles
</commit_message>
<xml_diff>
--- a/Combinations.xlsx
+++ b/Combinations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C46951E-0961-4AA9-B697-C6D9FCE21FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942B91BB-1308-4644-ACC6-BEBB52F3D00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A009557A-D0E6-45B8-942A-C4AB4B72D0E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="196">
   <si>
     <t>Input Variables</t>
   </si>
@@ -600,6 +600,30 @@
   </si>
   <si>
     <t>POA Pyr, monthly albedo</t>
+  </si>
+  <si>
+    <t>IEC1B</t>
+  </si>
+  <si>
+    <t>IEC2Mono</t>
+  </si>
+  <si>
+    <t>IEC2A</t>
+  </si>
+  <si>
+    <t>IEC2B</t>
+  </si>
+  <si>
+    <t>5-minute data - refmod</t>
+  </si>
+  <si>
+    <t>5-minute data - POA+BOA</t>
+  </si>
+  <si>
+    <t>5-minute data POA</t>
+  </si>
+  <si>
+    <t>5-minute data GHI+DHI</t>
   </si>
 </sst>
 </file>
@@ -934,6 +958,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -942,9 +972,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -966,9 +993,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -993,9 +1017,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1033,7 +1057,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1139,7 +1163,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1281,7 +1305,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1289,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F903F77-CC72-401E-A0BD-CC4B63665887}">
-  <dimension ref="A1:V73"/>
+  <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1359,12 +1383,12 @@
       <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
     </row>
     <row r="2" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
@@ -1722,40 +1746,40 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="24"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="25"/>
       <c r="N20" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="O20" s="21" t="s">
+      <c r="O20" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
       <c r="R20" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="S20" s="16" t="s">
+      <c r="S20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="18"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="20"/>
     </row>
     <row r="21" spans="1:22" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
@@ -1953,7 +1977,7 @@
       <c r="C24" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="16" t="s">
         <v>100</v>
       </c>
       <c r="E24" t="s">
@@ -2018,7 +2042,7 @@
       <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="19"/>
+      <c r="D25" s="16"/>
       <c r="E25" t="s">
         <v>27</v>
       </c>
@@ -2081,7 +2105,7 @@
       <c r="C26" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="19"/>
+      <c r="D26" s="16"/>
       <c r="E26" t="s">
         <v>27</v>
       </c>
@@ -2144,7 +2168,7 @@
       <c r="C27" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="16"/>
       <c r="E27" t="s">
         <v>27</v>
       </c>
@@ -2207,7 +2231,7 @@
       <c r="C28" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E28" t="s">
@@ -2272,7 +2296,7 @@
       <c r="C29" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="19"/>
+      <c r="D29" s="16"/>
       <c r="E29" t="s">
         <v>27</v>
       </c>
@@ -2335,7 +2359,7 @@
       <c r="C30" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="16"/>
       <c r="E30" t="s">
         <v>27</v>
       </c>
@@ -2398,7 +2422,7 @@
       <c r="C31" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="16" t="s">
         <v>111</v>
       </c>
       <c r="E31" t="s">
@@ -2463,7 +2487,7 @@
       <c r="C32" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="16"/>
       <c r="E32" t="s">
         <v>27</v>
       </c>
@@ -2526,7 +2550,7 @@
       <c r="C33" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="16"/>
       <c r="E33" t="s">
         <v>27</v>
       </c>
@@ -2589,7 +2613,7 @@
       <c r="C34" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="16"/>
       <c r="E34" t="s">
         <v>27</v>
       </c>
@@ -2652,7 +2676,7 @@
       <c r="C35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="17" t="s">
         <v>118</v>
       </c>
       <c r="E35" t="s">
@@ -2717,7 +2741,7 @@
       <c r="C36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="27"/>
+      <c r="D36" s="17"/>
       <c r="E36" t="s">
         <v>27</v>
       </c>
@@ -2780,7 +2804,7 @@
       <c r="C37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="27"/>
+      <c r="D37" s="17"/>
       <c r="E37" t="s">
         <v>27</v>
       </c>
@@ -2843,7 +2867,7 @@
       <c r="C38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="27"/>
+      <c r="D38" s="17"/>
       <c r="E38" t="s">
         <v>27</v>
       </c>
@@ -2906,7 +2930,7 @@
       <c r="C39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="27"/>
+      <c r="D39" s="17"/>
       <c r="E39" t="s">
         <v>27</v>
       </c>
@@ -2969,7 +2993,7 @@
       <c r="C40" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="27"/>
+      <c r="D40" s="17"/>
       <c r="E40" t="s">
         <v>27</v>
       </c>
@@ -3032,7 +3056,7 @@
       <c r="C41" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="16" t="s">
         <v>124</v>
       </c>
       <c r="E41" t="s">
@@ -3097,7 +3121,7 @@
       <c r="C42" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="19"/>
+      <c r="D42" s="16"/>
       <c r="E42" t="s">
         <v>27</v>
       </c>
@@ -3160,7 +3184,7 @@
       <c r="C43" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="19"/>
+      <c r="D43" s="16"/>
       <c r="E43" t="s">
         <v>27</v>
       </c>
@@ -3223,7 +3247,7 @@
       <c r="C44" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="19"/>
+      <c r="D44" s="16"/>
       <c r="E44" t="s">
         <v>27</v>
       </c>
@@ -3286,7 +3310,7 @@
       <c r="C45" t="s">
         <v>126</v>
       </c>
-      <c r="D45" s="19"/>
+      <c r="D45" s="16"/>
       <c r="E45" t="s">
         <v>27</v>
       </c>
@@ -3349,7 +3373,7 @@
       <c r="C46" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="19"/>
+      <c r="D46" s="16"/>
       <c r="E46" t="s">
         <v>27</v>
       </c>
@@ -3412,7 +3436,7 @@
       <c r="C47" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="19"/>
+      <c r="D47" s="16"/>
       <c r="E47" t="s">
         <v>27</v>
       </c>
@@ -3475,7 +3499,7 @@
       <c r="C48" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="D48" s="16" t="s">
         <v>123</v>
       </c>
       <c r="E48" t="s">
@@ -3540,7 +3564,7 @@
       <c r="C49" t="s">
         <v>130</v>
       </c>
-      <c r="D49" s="19"/>
+      <c r="D49" s="16"/>
       <c r="E49" t="s">
         <v>27</v>
       </c>
@@ -3603,7 +3627,7 @@
       <c r="C50" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="19"/>
+      <c r="D50" s="16"/>
       <c r="E50" t="s">
         <v>27</v>
       </c>
@@ -3666,7 +3690,7 @@
       <c r="C51" t="s">
         <v>131</v>
       </c>
-      <c r="D51" s="19"/>
+      <c r="D51" s="16"/>
       <c r="E51" t="s">
         <v>27</v>
       </c>
@@ -3794,7 +3818,7 @@
       <c r="C53" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="16" t="s">
         <v>134</v>
       </c>
       <c r="E53" t="s">
@@ -3859,7 +3883,7 @@
       <c r="C54" t="s">
         <v>136</v>
       </c>
-      <c r="D54" s="19"/>
+      <c r="D54" s="16"/>
       <c r="E54" t="s">
         <v>27</v>
       </c>
@@ -3922,7 +3946,7 @@
       <c r="C55" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="19"/>
+      <c r="D55" s="16"/>
       <c r="E55" t="s">
         <v>27</v>
       </c>
@@ -3985,7 +4009,7 @@
       <c r="C56" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="19"/>
+      <c r="D56" s="16"/>
       <c r="E56" t="s">
         <v>27</v>
       </c>
@@ -4048,7 +4072,7 @@
       <c r="C57" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="19"/>
+      <c r="D57" s="16"/>
       <c r="E57" t="s">
         <v>27</v>
       </c>
@@ -4111,7 +4135,7 @@
       <c r="C58" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="19"/>
+      <c r="D58" s="16"/>
       <c r="E58" t="s">
         <v>27</v>
       </c>
@@ -4174,7 +4198,7 @@
       <c r="C59" t="s">
         <v>144</v>
       </c>
-      <c r="D59" s="19"/>
+      <c r="D59" s="16"/>
       <c r="E59" t="s">
         <v>27</v>
       </c>
@@ -4237,7 +4261,7 @@
       <c r="C60" t="s">
         <v>140</v>
       </c>
-      <c r="D60" s="19"/>
+      <c r="D60" s="16"/>
       <c r="E60" t="s">
         <v>27</v>
       </c>
@@ -4300,7 +4324,7 @@
       <c r="C61" t="s">
         <v>141</v>
       </c>
-      <c r="D61" s="19"/>
+      <c r="D61" s="16"/>
       <c r="E61" t="s">
         <v>27</v>
       </c>
@@ -4363,7 +4387,7 @@
       <c r="C62" t="s">
         <v>142</v>
       </c>
-      <c r="D62" s="19"/>
+      <c r="D62" s="16"/>
       <c r="E62" t="s">
         <v>27</v>
       </c>
@@ -4426,7 +4450,7 @@
       <c r="C63" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="19"/>
+      <c r="D63" s="16"/>
       <c r="E63" t="s">
         <v>27</v>
       </c>
@@ -4489,7 +4513,7 @@
       <c r="C64" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="19"/>
+      <c r="D64" s="16"/>
       <c r="E64" t="s">
         <v>27</v>
       </c>
@@ -4552,7 +4576,7 @@
       <c r="C65" t="s">
         <v>147</v>
       </c>
-      <c r="D65" s="19"/>
+      <c r="D65" s="16"/>
       <c r="E65" t="s">
         <v>27</v>
       </c>
@@ -4615,7 +4639,7 @@
       <c r="C66" t="s">
         <v>148</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="D66" s="16" t="s">
         <v>157</v>
       </c>
       <c r="E66" t="s">
@@ -4680,7 +4704,7 @@
       <c r="C67" t="s">
         <v>149</v>
       </c>
-      <c r="D67" s="19"/>
+      <c r="D67" s="16"/>
       <c r="E67" t="s">
         <v>27</v>
       </c>
@@ -4743,7 +4767,7 @@
       <c r="C68" t="s">
         <v>153</v>
       </c>
-      <c r="D68" s="19"/>
+      <c r="D68" s="16"/>
       <c r="E68" t="s">
         <v>27</v>
       </c>
@@ -4806,7 +4830,7 @@
       <c r="C69" t="s">
         <v>154</v>
       </c>
-      <c r="D69" s="19"/>
+      <c r="D69" s="16"/>
       <c r="E69" t="s">
         <v>27</v>
       </c>
@@ -4869,7 +4893,7 @@
       <c r="C70" t="s">
         <v>155</v>
       </c>
-      <c r="D70" s="19" t="s">
+      <c r="D70" s="16" t="s">
         <v>158</v>
       </c>
       <c r="E70" t="s">
@@ -4934,7 +4958,7 @@
       <c r="C71" t="s">
         <v>156</v>
       </c>
-      <c r="D71" s="19"/>
+      <c r="D71" s="16"/>
       <c r="E71" t="s">
         <v>27</v>
       </c>
@@ -5117,13 +5141,268 @@
         <v>105</v>
       </c>
     </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D74" t="s">
+        <v>195</v>
+      </c>
+      <c r="E74" t="s">
+        <v>27</v>
+      </c>
+      <c r="F74" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H74" s="6">
+        <v>0</v>
+      </c>
+      <c r="I74" s="6">
+        <v>0</v>
+      </c>
+      <c r="J74" s="6">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>2</v>
+      </c>
+      <c r="P74">
+        <v>2</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>17</v>
+      </c>
+      <c r="S74" t="s">
+        <v>24</v>
+      </c>
+      <c r="T74" t="s">
+        <v>24</v>
+      </c>
+      <c r="U74" t="s">
+        <v>24</v>
+      </c>
+      <c r="V74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>1</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D75" t="s">
+        <v>194</v>
+      </c>
+      <c r="E75" t="s">
+        <v>27</v>
+      </c>
+      <c r="F75" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H75" s="6">
+        <v>0</v>
+      </c>
+      <c r="I75" s="6">
+        <v>0</v>
+      </c>
+      <c r="J75" s="6">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75">
+        <v>4</v>
+      </c>
+      <c r="P75">
+        <v>2</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>17</v>
+      </c>
+      <c r="S75" t="s">
+        <v>24</v>
+      </c>
+      <c r="T75" t="s">
+        <v>24</v>
+      </c>
+      <c r="U75" t="s">
+        <v>24</v>
+      </c>
+      <c r="V75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D76" t="s">
+        <v>193</v>
+      </c>
+      <c r="E76" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H76" s="6">
+        <v>0</v>
+      </c>
+      <c r="I76" s="6">
+        <v>0</v>
+      </c>
+      <c r="J76" s="6">
+        <v>2</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>4</v>
+      </c>
+      <c r="P76">
+        <v>2</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>17</v>
+      </c>
+      <c r="S76" t="s">
+        <v>24</v>
+      </c>
+      <c r="T76" t="s">
+        <v>24</v>
+      </c>
+      <c r="U76" t="s">
+        <v>24</v>
+      </c>
+      <c r="V76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D77" t="s">
+        <v>192</v>
+      </c>
+      <c r="E77" t="s">
+        <v>27</v>
+      </c>
+      <c r="F77" t="s">
+        <v>28</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H77" s="6">
+        <v>0</v>
+      </c>
+      <c r="I77" s="6">
+        <v>0</v>
+      </c>
+      <c r="J77" s="6">
+        <v>2</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>4</v>
+      </c>
+      <c r="P77">
+        <v>2</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>17</v>
+      </c>
+      <c r="S77" t="s">
+        <v>24</v>
+      </c>
+      <c r="T77" t="s">
+        <v>24</v>
+      </c>
+      <c r="U77" t="s">
+        <v>24</v>
+      </c>
+      <c r="V77" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="D41:D47"/>
     <mergeCell ref="S20:V20"/>
     <mergeCell ref="D53:D65"/>
     <mergeCell ref="D66:D69"/>
@@ -5133,6 +5412,11 @@
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="D28:D30"/>
     <mergeCell ref="A20:D20"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="D41:D47"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Method 2b temp correct
</commit_message>
<xml_diff>
--- a/Combinations.xlsx
+++ b/Combinations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdeline\Documents\Python Scripts\2022_Bifacial_irradiance_paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942B91BB-1308-4644-ACC6-BEBB52F3D00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791825BE-4457-4BAC-87B1-EFA328152D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A009557A-D0E6-45B8-942A-C4AB4B72D0E6}"/>
   </bookViews>
@@ -611,9 +611,6 @@
     <t>IEC2A</t>
   </si>
   <si>
-    <t>IEC2B</t>
-  </si>
-  <si>
     <t>5-minute data - refmod</t>
   </si>
   <si>
@@ -624,6 +621,9 @@
   </si>
   <si>
     <t>5-minute data GHI+DHI</t>
+  </si>
+  <si>
+    <t>IEC2B_tcorr</t>
   </si>
 </sst>
 </file>
@@ -958,12 +958,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -972,6 +966,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -993,6 +990,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1315,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F903F77-CC72-401E-A0BD-CC4B63665887}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1383,12 +1383,12 @@
       <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
     </row>
     <row r="2" spans="4:22" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
@@ -1746,40 +1746,40 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="24"/>
       <c r="N20" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="O20" s="22" t="s">
+      <c r="O20" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
       <c r="R20" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="S20" s="18" t="s">
+      <c r="S20" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="20"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="18"/>
     </row>
     <row r="21" spans="1:22" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
@@ -1977,7 +1977,7 @@
       <c r="C24" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="19" t="s">
         <v>100</v>
       </c>
       <c r="E24" t="s">
@@ -2042,7 +2042,7 @@
       <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="16"/>
+      <c r="D25" s="19"/>
       <c r="E25" t="s">
         <v>27</v>
       </c>
@@ -2105,7 +2105,7 @@
       <c r="C26" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="19"/>
       <c r="E26" t="s">
         <v>27</v>
       </c>
@@ -2168,7 +2168,7 @@
       <c r="C27" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="16"/>
+      <c r="D27" s="19"/>
       <c r="E27" t="s">
         <v>27</v>
       </c>
@@ -2231,7 +2231,7 @@
       <c r="C28" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="19" t="s">
         <v>110</v>
       </c>
       <c r="E28" t="s">
@@ -2296,7 +2296,7 @@
       <c r="C29" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="16"/>
+      <c r="D29" s="19"/>
       <c r="E29" t="s">
         <v>27</v>
       </c>
@@ -2359,7 +2359,7 @@
       <c r="C30" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="16"/>
+      <c r="D30" s="19"/>
       <c r="E30" t="s">
         <v>27</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="C31" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="19" t="s">
         <v>111</v>
       </c>
       <c r="E31" t="s">
@@ -2487,7 +2487,7 @@
       <c r="C32" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="16"/>
+      <c r="D32" s="19"/>
       <c r="E32" t="s">
         <v>27</v>
       </c>
@@ -2550,7 +2550,7 @@
       <c r="C33" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="16"/>
+      <c r="D33" s="19"/>
       <c r="E33" t="s">
         <v>27</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="C34" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="16"/>
+      <c r="D34" s="19"/>
       <c r="E34" t="s">
         <v>27</v>
       </c>
@@ -2676,7 +2676,7 @@
       <c r="C35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="27" t="s">
         <v>118</v>
       </c>
       <c r="E35" t="s">
@@ -2741,7 +2741,7 @@
       <c r="C36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="17"/>
+      <c r="D36" s="27"/>
       <c r="E36" t="s">
         <v>27</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="C37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="17"/>
+      <c r="D37" s="27"/>
       <c r="E37" t="s">
         <v>27</v>
       </c>
@@ -2867,7 +2867,7 @@
       <c r="C38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="17"/>
+      <c r="D38" s="27"/>
       <c r="E38" t="s">
         <v>27</v>
       </c>
@@ -2930,7 +2930,7 @@
       <c r="C39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="27"/>
       <c r="E39" t="s">
         <v>27</v>
       </c>
@@ -2993,7 +2993,7 @@
       <c r="C40" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="17"/>
+      <c r="D40" s="27"/>
       <c r="E40" t="s">
         <v>27</v>
       </c>
@@ -3056,7 +3056,7 @@
       <c r="C41" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="19" t="s">
         <v>124</v>
       </c>
       <c r="E41" t="s">
@@ -3121,7 +3121,7 @@
       <c r="C42" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="16"/>
+      <c r="D42" s="19"/>
       <c r="E42" t="s">
         <v>27</v>
       </c>
@@ -3184,7 +3184,7 @@
       <c r="C43" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="16"/>
+      <c r="D43" s="19"/>
       <c r="E43" t="s">
         <v>27</v>
       </c>
@@ -3247,7 +3247,7 @@
       <c r="C44" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="16"/>
+      <c r="D44" s="19"/>
       <c r="E44" t="s">
         <v>27</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c r="C45" t="s">
         <v>126</v>
       </c>
-      <c r="D45" s="16"/>
+      <c r="D45" s="19"/>
       <c r="E45" t="s">
         <v>27</v>
       </c>
@@ -3373,7 +3373,7 @@
       <c r="C46" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="16"/>
+      <c r="D46" s="19"/>
       <c r="E46" t="s">
         <v>27</v>
       </c>
@@ -3436,7 +3436,7 @@
       <c r="C47" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="16"/>
+      <c r="D47" s="19"/>
       <c r="E47" t="s">
         <v>27</v>
       </c>
@@ -3499,7 +3499,7 @@
       <c r="C48" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="19" t="s">
         <v>123</v>
       </c>
       <c r="E48" t="s">
@@ -3564,7 +3564,7 @@
       <c r="C49" t="s">
         <v>130</v>
       </c>
-      <c r="D49" s="16"/>
+      <c r="D49" s="19"/>
       <c r="E49" t="s">
         <v>27</v>
       </c>
@@ -3627,7 +3627,7 @@
       <c r="C50" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="16"/>
+      <c r="D50" s="19"/>
       <c r="E50" t="s">
         <v>27</v>
       </c>
@@ -3690,7 +3690,7 @@
       <c r="C51" t="s">
         <v>131</v>
       </c>
-      <c r="D51" s="16"/>
+      <c r="D51" s="19"/>
       <c r="E51" t="s">
         <v>27</v>
       </c>
@@ -3818,7 +3818,7 @@
       <c r="C53" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="19" t="s">
         <v>134</v>
       </c>
       <c r="E53" t="s">
@@ -3883,7 +3883,7 @@
       <c r="C54" t="s">
         <v>136</v>
       </c>
-      <c r="D54" s="16"/>
+      <c r="D54" s="19"/>
       <c r="E54" t="s">
         <v>27</v>
       </c>
@@ -3946,7 +3946,7 @@
       <c r="C55" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="16"/>
+      <c r="D55" s="19"/>
       <c r="E55" t="s">
         <v>27</v>
       </c>
@@ -4009,7 +4009,7 @@
       <c r="C56" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="16"/>
+      <c r="D56" s="19"/>
       <c r="E56" t="s">
         <v>27</v>
       </c>
@@ -4072,7 +4072,7 @@
       <c r="C57" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="16"/>
+      <c r="D57" s="19"/>
       <c r="E57" t="s">
         <v>27</v>
       </c>
@@ -4135,7 +4135,7 @@
       <c r="C58" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="16"/>
+      <c r="D58" s="19"/>
       <c r="E58" t="s">
         <v>27</v>
       </c>
@@ -4198,7 +4198,7 @@
       <c r="C59" t="s">
         <v>144</v>
       </c>
-      <c r="D59" s="16"/>
+      <c r="D59" s="19"/>
       <c r="E59" t="s">
         <v>27</v>
       </c>
@@ -4261,7 +4261,7 @@
       <c r="C60" t="s">
         <v>140</v>
       </c>
-      <c r="D60" s="16"/>
+      <c r="D60" s="19"/>
       <c r="E60" t="s">
         <v>27</v>
       </c>
@@ -4324,7 +4324,7 @@
       <c r="C61" t="s">
         <v>141</v>
       </c>
-      <c r="D61" s="16"/>
+      <c r="D61" s="19"/>
       <c r="E61" t="s">
         <v>27</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="C62" t="s">
         <v>142</v>
       </c>
-      <c r="D62" s="16"/>
+      <c r="D62" s="19"/>
       <c r="E62" t="s">
         <v>27</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="C63" t="s">
         <v>145</v>
       </c>
-      <c r="D63" s="16"/>
+      <c r="D63" s="19"/>
       <c r="E63" t="s">
         <v>27</v>
       </c>
@@ -4513,7 +4513,7 @@
       <c r="C64" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="16"/>
+      <c r="D64" s="19"/>
       <c r="E64" t="s">
         <v>27</v>
       </c>
@@ -4576,7 +4576,7 @@
       <c r="C65" t="s">
         <v>147</v>
       </c>
-      <c r="D65" s="16"/>
+      <c r="D65" s="19"/>
       <c r="E65" t="s">
         <v>27</v>
       </c>
@@ -4639,7 +4639,7 @@
       <c r="C66" t="s">
         <v>148</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="19" t="s">
         <v>157</v>
       </c>
       <c r="E66" t="s">
@@ -4704,7 +4704,7 @@
       <c r="C67" t="s">
         <v>149</v>
       </c>
-      <c r="D67" s="16"/>
+      <c r="D67" s="19"/>
       <c r="E67" t="s">
         <v>27</v>
       </c>
@@ -4767,7 +4767,7 @@
       <c r="C68" t="s">
         <v>153</v>
       </c>
-      <c r="D68" s="16"/>
+      <c r="D68" s="19"/>
       <c r="E68" t="s">
         <v>27</v>
       </c>
@@ -4830,7 +4830,7 @@
       <c r="C69" t="s">
         <v>154</v>
       </c>
-      <c r="D69" s="16"/>
+      <c r="D69" s="19"/>
       <c r="E69" t="s">
         <v>27</v>
       </c>
@@ -4893,7 +4893,7 @@
       <c r="C70" t="s">
         <v>155</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D70" s="19" t="s">
         <v>158</v>
       </c>
       <c r="E70" t="s">
@@ -4958,7 +4958,7 @@
       <c r="C71" t="s">
         <v>156</v>
       </c>
-      <c r="D71" s="16"/>
+      <c r="D71" s="19"/>
       <c r="E71" t="s">
         <v>27</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>188</v>
       </c>
       <c r="D74" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E74" t="s">
         <v>27</v>
@@ -5217,7 +5217,7 @@
         <v>189</v>
       </c>
       <c r="D75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E75" t="s">
         <v>27</v>
@@ -5282,7 +5282,7 @@
         <v>190</v>
       </c>
       <c r="D76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E76" t="s">
         <v>27</v>
@@ -5341,13 +5341,13 @@
         <v>1</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" t="s">
         <v>191</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D77" t="s">
-        <v>192</v>
       </c>
       <c r="E77" t="s">
         <v>27</v>
@@ -5403,6 +5403,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="D41:D47"/>
     <mergeCell ref="S20:V20"/>
     <mergeCell ref="D53:D65"/>
     <mergeCell ref="D66:D69"/>
@@ -5412,11 +5417,6 @@
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="D28:D30"/>
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="D41:D47"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>